<commit_message>
VACCINECERT-1633 Fixed CSV upload templates
</commit_message>
<xml_diff>
--- a/template-cc_antibody-delivery_appTransfer.xlsx
+++ b/template-cc_antibody-delivery_appTransfer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\adb.intra.admin.ch\Userhome$\All\config\Desktop\template-cc_antibody\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80845697\Downloads\template-cc_antibody-delivery_appTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22596" windowHeight="5148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13605"/>
   </bookViews>
   <sheets>
     <sheet name="vaccination-appTransfer" sheetId="3" r:id="rId1"/>
@@ -546,48 +546,48 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -902,21 +902,21 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.34765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.84765625" style="1"/>
-    <col min="4" max="4" width="8.6484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.34765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
+    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -953,7 +953,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>44501</v>
+        <v>44516</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>

</xml_diff>